<commit_message>
Code to handle dates integrated into build_functions
</commit_message>
<xml_diff>
--- a/CV.xlsx
+++ b/CV.xlsx
@@ -1966,7 +1966,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1988,6 +1988,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1995,12 +1999,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -2119,7 +2123,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="1" sqref="A22:F23 D3"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2296,7 +2300,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A22:F23 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2326,7 +2330,7 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9" t="n">
+      <c r="A2" s="10" t="n">
         <v>20140901</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -2350,7 +2354,7 @@
       <c r="H2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="n">
+      <c r="A3" s="10" t="n">
         <v>20140501</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -2374,7 +2378,7 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9" t="n">
+      <c r="A4" s="10" t="n">
         <v>20130801</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -2398,7 +2402,7 @@
       <c r="H4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9" t="n">
+      <c r="A5" s="10" t="n">
         <v>20130501</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -2532,7 +2536,7 @@
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A22:F23 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2585,12 +2589,12 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B3" activeCellId="1" sqref="A22:F23 B3"/>
+      <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="6" width="20.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="20.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3168,7 +3172,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A22:F23 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3211,10 +3215,10 @@
       <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="16" t="n">
+      <c r="C3" s="17" t="n">
         <v>44774</v>
       </c>
-      <c r="D3" s="16" t="n">
+      <c r="D3" s="17" t="n">
         <v>45047</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -3228,10 +3232,10 @@
       <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="16" t="n">
+      <c r="C4" s="17" t="n">
         <v>44774</v>
       </c>
-      <c r="D4" s="16" t="n">
+      <c r="D4" s="17" t="n">
         <v>45047</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -3245,10 +3249,10 @@
       <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="17" t="n">
+      <c r="C5" s="18" t="n">
         <v>44835</v>
       </c>
-      <c r="D5" s="16" t="n">
+      <c r="D5" s="17" t="n">
         <v>45047</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -3262,7 +3266,7 @@
       <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="16" t="n">
+      <c r="C6" s="17" t="n">
         <v>44409</v>
       </c>
       <c r="E6" s="1" t="s">
@@ -3288,9 +3292,9 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F22" activeCellId="0" sqref="A22:F23"/>
+      <selection pane="bottomLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3325,7 +3329,7 @@
       <c r="A2" s="1" t="s">
         <v>516</v>
       </c>
-      <c r="B2" s="8" t="b">
+      <c r="B2" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3349,7 +3353,7 @@
       <c r="A3" s="1" t="s">
         <v>516</v>
       </c>
-      <c r="B3" s="8" t="b">
+      <c r="B3" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3373,7 +3377,7 @@
       <c r="A4" s="1" t="s">
         <v>516</v>
       </c>
-      <c r="B4" s="8" t="b">
+      <c r="B4" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -3400,7 +3404,7 @@
       <c r="A5" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="B5" s="8" t="b">
+      <c r="B5" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3427,7 +3431,7 @@
       <c r="A6" s="1" t="s">
         <v>516</v>
       </c>
-      <c r="B6" s="8" t="b">
+      <c r="B6" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3448,7 +3452,7 @@
       <c r="A7" s="1" t="s">
         <v>516</v>
       </c>
-      <c r="B7" s="8" t="b">
+      <c r="B7" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3472,7 +3476,7 @@
       <c r="A8" s="1" t="s">
         <v>516</v>
       </c>
-      <c r="B8" s="8" t="b">
+      <c r="B8" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3493,7 +3497,7 @@
       <c r="A9" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="B9" s="8" t="b">
+      <c r="B9" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3517,7 +3521,7 @@
       <c r="A10" s="1" t="s">
         <v>534</v>
       </c>
-      <c r="B10" s="8" t="b">
+      <c r="B10" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -3541,7 +3545,7 @@
       <c r="A11" s="1" t="s">
         <v>516</v>
       </c>
-      <c r="B11" s="8" t="b">
+      <c r="B11" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3562,7 +3566,7 @@
       <c r="A12" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="B12" s="8" t="b">
+      <c r="B12" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3589,7 +3593,7 @@
       <c r="A13" s="1" t="s">
         <v>534</v>
       </c>
-      <c r="B13" s="8" t="b">
+      <c r="B13" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3613,7 +3617,7 @@
       <c r="A14" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="B14" s="8" t="b">
+      <c r="B14" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3634,7 +3638,7 @@
       <c r="A15" s="1" t="s">
         <v>534</v>
       </c>
-      <c r="B15" s="8" t="b">
+      <c r="B15" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -3655,7 +3659,7 @@
       <c r="A16" s="1" t="s">
         <v>534</v>
       </c>
-      <c r="B16" s="8" t="b">
+      <c r="B16" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -3679,7 +3683,7 @@
       <c r="A17" s="1" t="s">
         <v>516</v>
       </c>
-      <c r="B17" s="8" t="b">
+      <c r="B17" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3703,7 +3707,7 @@
       <c r="A18" s="1" t="s">
         <v>534</v>
       </c>
-      <c r="B18" s="8" t="b">
+      <c r="B18" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3727,7 +3731,7 @@
       <c r="A19" s="1" t="s">
         <v>516</v>
       </c>
-      <c r="B19" s="8" t="b">
+      <c r="B19" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3751,7 +3755,7 @@
       <c r="A20" s="1" t="s">
         <v>516</v>
       </c>
-      <c r="B20" s="8" t="b">
+      <c r="B20" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3771,11 +3775,11 @@
         <v>518</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
         <v>534</v>
       </c>
-      <c r="B21" s="1" t="b">
+      <c r="B21" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3822,7 +3826,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A22:F23 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3998,7 +4002,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A22:F23 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4027,7 +4031,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="b">
+      <c r="A2" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -4045,7 +4049,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="b">
+      <c r="A3" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4063,7 +4067,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="b">
+      <c r="A4" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4081,7 +4085,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="b">
+      <c r="A5" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -4096,7 +4100,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="b">
+      <c r="A6" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -4132,7 +4136,7 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A22:F23 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4170,17 +4174,17 @@
       <c r="L1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="b">
+      <c r="A2" s="6" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>580</v>
       </c>
-      <c r="C2" s="9" t="n">
+      <c r="C2" s="10" t="n">
         <v>2023</v>
       </c>
-      <c r="D2" s="9" t="n">
+      <c r="D2" s="10" t="n">
         <v>2023</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -4198,17 +4202,17 @@
       <c r="L2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="b">
+      <c r="A3" s="6" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>580</v>
       </c>
-      <c r="C3" s="9" t="n">
+      <c r="C3" s="10" t="n">
         <v>2022</v>
       </c>
-      <c r="D3" s="9" t="n">
+      <c r="D3" s="10" t="n">
         <v>2022</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -4226,17 +4230,17 @@
       <c r="L3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="b">
+      <c r="A4" s="6" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>580</v>
       </c>
-      <c r="C4" s="9" t="n">
+      <c r="C4" s="10" t="n">
         <v>2022</v>
       </c>
-      <c r="D4" s="9" t="n">
+      <c r="D4" s="10" t="n">
         <v>2022</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -4254,17 +4258,17 @@
       <c r="L4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="b">
+      <c r="A5" s="6" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>580</v>
       </c>
-      <c r="C5" s="9" t="n">
+      <c r="C5" s="10" t="n">
         <v>2022</v>
       </c>
-      <c r="D5" s="9" t="n">
+      <c r="D5" s="10" t="n">
         <v>2022</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -4282,17 +4286,17 @@
       <c r="L5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="b">
+      <c r="A6" s="6" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>580</v>
       </c>
-      <c r="C6" s="9" t="n">
+      <c r="C6" s="10" t="n">
         <v>2021</v>
       </c>
-      <c r="D6" s="9" t="n">
+      <c r="D6" s="10" t="n">
         <v>2021</v>
       </c>
       <c r="E6" s="1" t="s">
@@ -4311,17 +4315,17 @@
       <c r="L6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="b">
+      <c r="A7" s="6" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>592</v>
       </c>
-      <c r="C7" s="9" t="n">
+      <c r="C7" s="10" t="n">
         <v>2021</v>
       </c>
-      <c r="D7" s="9" t="n">
+      <c r="D7" s="10" t="n">
         <v>2021</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -4340,17 +4344,17 @@
       <c r="L7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="b">
+      <c r="A8" s="6" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>592</v>
       </c>
-      <c r="C8" s="9" t="n">
+      <c r="C8" s="10" t="n">
         <v>2021</v>
       </c>
-      <c r="D8" s="9" t="n">
+      <c r="D8" s="10" t="n">
         <v>2021</v>
       </c>
       <c r="E8" s="1" t="s">
@@ -4369,17 +4373,17 @@
       <c r="L8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="b">
+      <c r="A9" s="6" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>592</v>
       </c>
-      <c r="C9" s="9" t="n">
+      <c r="C9" s="10" t="n">
         <v>2020</v>
       </c>
-      <c r="D9" s="9" t="n">
+      <c r="D9" s="10" t="n">
         <v>2020</v>
       </c>
       <c r="E9" s="1" t="s">
@@ -4530,7 +4534,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A22:F23 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4619,7 +4623,7 @@
   <dimension ref="A1:AD11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="1" sqref="A22:F23 C9"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4675,14 +4679,14 @@
       <c r="AD1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="b">
+      <c r="A2" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="5" t="b">
+      <c r="C2" s="6" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4727,14 +4731,14 @@
       <c r="AD2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="b">
+      <c r="A3" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="5" t="b">
+      <c r="C3" s="6" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4775,14 +4779,14 @@
       <c r="AD3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="b">
+      <c r="A4" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="5" t="b">
+      <c r="C4" s="6" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4827,14 +4831,14 @@
       <c r="AD4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="b">
+      <c r="A5" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="5" t="b">
+      <c r="C5" s="6" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4879,14 +4883,14 @@
       <c r="AD5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="b">
+      <c r="A6" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="5" t="b">
+      <c r="C6" s="6" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4931,14 +4935,14 @@
       <c r="AD6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="b">
+      <c r="A7" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="5" t="b">
+      <c r="C7" s="6" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4983,14 +4987,14 @@
       <c r="AD7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="b">
+      <c r="A8" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="1" t="b">
+      <c r="C8" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -5031,14 +5035,14 @@
       <c r="AD8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="b">
+      <c r="A9" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="1" t="b">
+      <c r="C9" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5059,14 +5063,14 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="b">
+      <c r="A10" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="1" t="b">
+      <c r="C10" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -5087,14 +5091,14 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="b">
+      <c r="A11" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="1" t="b">
+      <c r="C11" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -5130,12 +5134,12 @@
   <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A22:F23 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="6" width="31.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="7" width="31.38"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5183,7 +5187,7 @@
       <c r="A2" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="1" t="b">
+      <c r="B2" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5205,7 +5209,7 @@
       <c r="H2" s="1" t="n">
         <v>299859</v>
       </c>
-      <c r="I2" s="1" t="b">
+      <c r="I2" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -5224,7 +5228,7 @@
       <c r="A3" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="1" t="b">
+      <c r="B3" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -5246,7 +5250,7 @@
       <c r="H3" s="1" t="n">
         <v>380650</v>
       </c>
-      <c r="I3" s="1" t="b">
+      <c r="I3" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5262,7 +5266,7 @@
       <c r="A4" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="1" t="b">
+      <c r="B4" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -5284,7 +5288,7 @@
       <c r="H4" s="1" t="n">
         <v>20000000</v>
       </c>
-      <c r="I4" s="1" t="b">
+      <c r="I4" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -5303,7 +5307,7 @@
       <c r="A5" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B5" s="1" t="b">
+      <c r="B5" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -5325,7 +5329,7 @@
       <c r="H5" s="1" t="n">
         <v>4000000</v>
       </c>
-      <c r="I5" s="1" t="b">
+      <c r="I5" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -5346,7 +5350,7 @@
       <c r="A6" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B6" s="1" t="b">
+      <c r="B6" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -5368,7 +5372,7 @@
       <c r="H6" s="1" t="n">
         <v>300000</v>
       </c>
-      <c r="I6" s="1" t="b">
+      <c r="I6" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5383,7 +5387,7 @@
       <c r="A7" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B7" s="1" t="b">
+      <c r="B7" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -5405,7 +5409,7 @@
       <c r="H7" s="1" t="n">
         <v>1500000</v>
       </c>
-      <c r="I7" s="1" t="b">
+      <c r="I7" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -5423,7 +5427,7 @@
       <c r="A8" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B8" s="1" t="b">
+      <c r="B8" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -5445,7 +5449,7 @@
       <c r="H8" s="1" t="n">
         <v>197699</v>
       </c>
-      <c r="I8" s="1" t="b">
+      <c r="I8" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -5463,7 +5467,7 @@
       <c r="A9" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B9" s="1" t="b">
+      <c r="B9" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5485,7 +5489,7 @@
       <c r="H9" s="1" t="n">
         <v>300000</v>
       </c>
-      <c r="I9" s="1" t="b">
+      <c r="I9" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5494,7 +5498,7 @@
       <c r="A10" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B10" s="1" t="b">
+      <c r="B10" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5516,7 +5520,7 @@
       <c r="H10" s="1" t="n">
         <v>20000000</v>
       </c>
-      <c r="I10" s="1" t="b">
+      <c r="I10" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5528,7 +5532,7 @@
       <c r="A11" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B11" s="1" t="b">
+      <c r="B11" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5550,7 +5554,7 @@
       <c r="H11" s="1" t="n">
         <v>3000000</v>
       </c>
-      <c r="I11" s="1" t="b">
+      <c r="I11" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5559,7 +5563,7 @@
       <c r="A12" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B12" s="1" t="b">
+      <c r="B12" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5581,7 +5585,7 @@
       <c r="H12" s="1" t="n">
         <v>281755</v>
       </c>
-      <c r="I12" s="1" t="b">
+      <c r="I12" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5590,7 +5594,7 @@
       <c r="A13" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B13" s="1" t="b">
+      <c r="B13" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5603,7 +5607,7 @@
       <c r="E13" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="8" t="s">
         <v>100</v>
       </c>
       <c r="G13" s="1" t="s">
@@ -5612,13 +5616,13 @@
       <c r="H13" s="1" t="n">
         <v>666485</v>
       </c>
-      <c r="I13" s="1" t="b">
+      <c r="I13" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F14" s="7"/>
+      <c r="F14" s="9"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -5639,7 +5643,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A22:F23 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5709,7 +5713,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="1" sqref="A22:F23 F1"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5741,21 +5745,21 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="b">
+      <c r="A2" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C2" s="5" t="b">
+      <c r="C2" s="6" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D2" s="9" t="n">
+      <c r="D2" s="10" t="n">
         <v>2021</v>
       </c>
-      <c r="E2" s="9" t="n">
+      <c r="E2" s="10" t="n">
         <v>2021</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -5764,26 +5768,26 @@
       <c r="G2" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="7" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="b">
+      <c r="A3" s="5" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C3" s="5" t="b">
+      <c r="C3" s="6" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D3" s="9" t="n">
+      <c r="D3" s="10" t="n">
         <v>2012</v>
       </c>
-      <c r="E3" s="9" t="n">
+      <c r="E3" s="10" t="n">
         <v>2012</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -5794,21 +5798,21 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="b">
+      <c r="A4" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C4" s="5" t="b">
+      <c r="C4" s="6" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="D4" s="9" t="n">
+      <c r="D4" s="10" t="n">
         <v>2009</v>
       </c>
-      <c r="E4" s="9" t="n">
+      <c r="E4" s="10" t="n">
         <v>2011</v>
       </c>
       <c r="F4" s="1" t="s">
@@ -5820,21 +5824,21 @@
       <c r="H4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="b">
+      <c r="A5" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C5" s="5" t="b">
+      <c r="C5" s="6" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="D5" s="9" t="n">
+      <c r="D5" s="10" t="n">
         <v>2005</v>
       </c>
-      <c r="E5" s="9" t="n">
+      <c r="E5" s="10" t="n">
         <v>2009</v>
       </c>
       <c r="F5" s="1" t="s">
@@ -5846,21 +5850,21 @@
       <c r="H5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="b">
+      <c r="A6" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C6" s="5" t="b">
+      <c r="C6" s="6" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D6" s="9" t="n">
+      <c r="D6" s="10" t="n">
         <v>2009</v>
       </c>
-      <c r="E6" s="9" t="n">
+      <c r="E6" s="10" t="n">
         <v>2009</v>
       </c>
       <c r="F6" s="1" t="s">
@@ -5872,21 +5876,21 @@
       <c r="H6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8" t="b">
+      <c r="A7" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C7" s="5" t="b">
+      <c r="C7" s="6" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D7" s="9" t="n">
+      <c r="D7" s="10" t="n">
         <v>2009</v>
       </c>
-      <c r="E7" s="9" t="n">
+      <c r="E7" s="10" t="n">
         <v>2009</v>
       </c>
       <c r="F7" s="1" t="s">
@@ -5898,21 +5902,21 @@
       <c r="H7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="b">
+      <c r="A8" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C8" s="5" t="b">
+      <c r="C8" s="6" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="D8" s="9" t="n">
+      <c r="D8" s="10" t="n">
         <v>2006</v>
       </c>
-      <c r="E8" s="9" t="n">
+      <c r="E8" s="10" t="n">
         <v>2009</v>
       </c>
       <c r="F8" s="1" t="s">
@@ -5924,21 +5928,21 @@
       <c r="H8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="b">
+      <c r="A9" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C9" s="5" t="b">
+      <c r="C9" s="6" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="D9" s="9" t="n">
+      <c r="D9" s="10" t="n">
         <v>2005</v>
       </c>
-      <c r="E9" s="9" t="n">
+      <c r="E9" s="10" t="n">
         <v>2009</v>
       </c>
       <c r="F9" s="1" t="s">
@@ -5950,21 +5954,21 @@
       <c r="H9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8" t="b">
+      <c r="A10" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C10" s="5" t="b">
+      <c r="C10" s="6" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D10" s="9" t="n">
+      <c r="D10" s="10" t="n">
         <v>2005</v>
       </c>
-      <c r="E10" s="9" t="n">
+      <c r="E10" s="10" t="n">
         <v>2005</v>
       </c>
       <c r="F10" s="1" t="s">
@@ -5976,21 +5980,21 @@
       <c r="H10" s="1"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8" t="b">
+      <c r="A11" s="5" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C11" s="5" t="b">
+      <c r="C11" s="6" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D11" s="9" t="n">
+      <c r="D11" s="10" t="n">
         <v>2005</v>
       </c>
-      <c r="E11" s="9" t="n">
+      <c r="E11" s="10" t="n">
         <v>2005</v>
       </c>
       <c r="F11" s="1" t="s">
@@ -6026,7 +6030,7 @@
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="10"/>
+      <c r="G14" s="11"/>
       <c r="H14" s="1"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6065,7 +6069,7 @@
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-      <c r="F18" s="10"/>
+      <c r="F18" s="11"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
@@ -6075,7 +6079,7 @@
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="10"/>
+      <c r="F19" s="11"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
     </row>
@@ -6098,7 +6102,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A22:F23 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6130,7 +6134,7 @@
       <c r="C2" s="1" t="n">
         <v>2021</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="12" t="s">
         <v>133</v>
       </c>
     </row>
@@ -6144,7 +6148,7 @@
       <c r="C3" s="1" t="n">
         <v>2020</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="12" t="s">
         <v>136</v>
       </c>
     </row>
@@ -6161,7 +6165,7 @@
       <c r="D4" s="1" t="n">
         <v>2021</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="12" t="s">
         <v>139</v>
       </c>
     </row>
@@ -6175,7 +6179,7 @@
       <c r="C5" s="1" t="n">
         <v>2019</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="12" t="s">
         <v>142</v>
       </c>
     </row>
@@ -6189,7 +6193,7 @@
       <c r="C6" s="1" t="n">
         <v>2018</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="12" t="s">
         <v>145</v>
       </c>
     </row>
@@ -6203,7 +6207,7 @@
       <c r="C7" s="1" t="n">
         <v>2018</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="12" t="s">
         <v>148</v>
       </c>
     </row>
@@ -6217,7 +6221,7 @@
       <c r="C8" s="1" t="n">
         <v>2018</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="12" t="s">
         <v>151</v>
       </c>
     </row>
@@ -6234,7 +6238,7 @@
       <c r="D9" s="1" t="n">
         <v>2020</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="12" t="s">
         <v>154</v>
       </c>
     </row>
@@ -6251,7 +6255,7 @@
       <c r="D10" s="1" t="n">
         <v>2021</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="12" t="s">
         <v>157</v>
       </c>
     </row>
@@ -6268,7 +6272,7 @@
       <c r="D11" s="1" t="n">
         <v>2015</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="12" t="s">
         <v>160</v>
       </c>
     </row>
@@ -6305,14 +6309,14 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G12" activeCellId="1" sqref="A22:F23 G12"/>
+      <selection pane="bottomLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="6" width="68.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="6" width="14.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="6" width="113.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="68.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="7" width="14.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="7" width="113.88"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6404,13 +6408,13 @@
       <c r="H3" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="J3" s="12" t="s">
         <v>182</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="L3" s="11" t="s">
+      <c r="L3" s="12" t="s">
         <v>184</v>
       </c>
     </row>
@@ -6439,13 +6443,13 @@
       <c r="H4" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="J4" s="11" t="s">
+      <c r="J4" s="12" t="s">
         <v>188</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="L4" s="11" t="s">
+      <c r="L4" s="12" t="s">
         <v>190</v>
       </c>
     </row>
@@ -6474,16 +6478,16 @@
       <c r="H5" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="I5" s="12" t="s">
+      <c r="I5" s="13" t="s">
         <v>193</v>
       </c>
-      <c r="J5" s="11" t="s">
+      <c r="J5" s="12" t="s">
         <v>194</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="L5" s="11" t="s">
+      <c r="L5" s="12" t="s">
         <v>196</v>
       </c>
     </row>
@@ -6515,13 +6519,13 @@
       <c r="I6" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="J6" s="11" t="s">
+      <c r="J6" s="12" t="s">
         <v>201</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="L6" s="11" t="s">
+      <c r="L6" s="12" t="s">
         <v>202</v>
       </c>
     </row>
@@ -6579,16 +6583,16 @@
       <c r="H8" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="I8" s="13" t="s">
+      <c r="I8" s="14" t="s">
         <v>209</v>
       </c>
-      <c r="J8" s="11" t="s">
+      <c r="J8" s="12" t="s">
         <v>210</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="L8" s="11" t="s">
+      <c r="L8" s="12" t="s">
         <v>212</v>
       </c>
     </row>
@@ -6646,16 +6650,16 @@
       <c r="H10" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="I10" s="13" t="s">
+      <c r="I10" s="14" t="s">
         <v>209</v>
       </c>
-      <c r="J10" s="11" t="s">
+      <c r="J10" s="12" t="s">
         <v>219</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="L10" s="11" t="s">
+      <c r="L10" s="12" t="s">
         <v>220</v>
       </c>
     </row>
@@ -6687,13 +6691,13 @@
       <c r="I11" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="J11" s="11" t="s">
+      <c r="J11" s="12" t="s">
         <v>224</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="L11" s="11" t="s">
+      <c r="L11" s="12" t="s">
         <v>226</v>
       </c>
     </row>
@@ -6725,13 +6729,13 @@
       <c r="I12" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="J12" s="11" t="s">
+      <c r="J12" s="12" t="s">
         <v>230</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="L12" s="11" t="s">
+      <c r="L12" s="12" t="s">
         <v>232</v>
       </c>
     </row>
@@ -6760,13 +6764,13 @@
       <c r="I13" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="J13" s="11" t="s">
+      <c r="J13" s="12" t="s">
         <v>237</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="L13" s="11" t="s">
+      <c r="L13" s="12" t="s">
         <v>239</v>
       </c>
     </row>
@@ -6795,13 +6799,13 @@
       <c r="H14" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="J14" s="11" t="s">
+      <c r="J14" s="12" t="s">
         <v>244</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="L14" s="11" t="s">
+      <c r="L14" s="12" t="s">
         <v>246</v>
       </c>
     </row>
@@ -6830,13 +6834,13 @@
       <c r="H15" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="J15" s="11" t="s">
+      <c r="J15" s="12" t="s">
         <v>252</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="L15" s="11" t="s">
+      <c r="L15" s="12" t="s">
         <v>254</v>
       </c>
     </row>
@@ -6868,13 +6872,13 @@
       <c r="I16" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="J16" s="11" t="s">
+      <c r="J16" s="12" t="s">
         <v>260</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="L16" s="11" t="s">
+      <c r="L16" s="12" t="s">
         <v>262</v>
       </c>
     </row>
@@ -6903,13 +6907,13 @@
       <c r="H17" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="J17" s="14" t="s">
+      <c r="J17" s="15" t="s">
         <v>266</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="L17" s="11" t="s">
+      <c r="L17" s="12" t="s">
         <v>268</v>
       </c>
     </row>
@@ -6935,13 +6939,13 @@
       <c r="H18" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="J18" s="14" t="s">
+      <c r="J18" s="15" t="s">
         <v>272</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="L18" s="11" t="s">
+      <c r="L18" s="12" t="s">
         <v>274</v>
       </c>
     </row>
@@ -6970,13 +6974,13 @@
       <c r="H19" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="J19" s="14" t="s">
+      <c r="J19" s="15" t="s">
         <v>277</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="L19" s="11" t="s">
+      <c r="L19" s="12" t="s">
         <v>279</v>
       </c>
     </row>
@@ -7008,13 +7012,13 @@
       <c r="I20" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="J20" s="14" t="s">
+      <c r="J20" s="15" t="s">
         <v>284</v>
       </c>
       <c r="K20" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="L20" s="11" t="s">
+      <c r="L20" s="12" t="s">
         <v>286</v>
       </c>
     </row>
@@ -7046,13 +7050,13 @@
       <c r="I21" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="J21" s="14" t="s">
+      <c r="J21" s="15" t="s">
         <v>292</v>
       </c>
       <c r="K21" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="L21" s="11" t="s">
+      <c r="L21" s="12" t="s">
         <v>294</v>
       </c>
     </row>
@@ -7084,13 +7088,13 @@
       <c r="I22" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="J22" s="14" t="s">
+      <c r="J22" s="15" t="s">
         <v>301</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="L22" s="11" t="s">
+      <c r="L22" s="12" t="s">
         <v>303</v>
       </c>
     </row>
@@ -7116,13 +7120,13 @@
       <c r="H23" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="J23" s="14" t="s">
+      <c r="J23" s="15" t="s">
         <v>306</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="L23" s="11" t="s">
+      <c r="L23" s="12" t="s">
         <v>307</v>
       </c>
     </row>
@@ -7154,13 +7158,13 @@
       <c r="I24" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="J24" s="14" t="s">
+      <c r="J24" s="15" t="s">
         <v>311</v>
       </c>
       <c r="K24" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="L24" s="11" t="s">
+      <c r="L24" s="12" t="s">
         <v>313</v>
       </c>
     </row>
@@ -7192,13 +7196,13 @@
       <c r="I25" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="J25" s="11" t="s">
+      <c r="J25" s="12" t="s">
         <v>315</v>
       </c>
       <c r="K25" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="L25" s="11" t="s">
+      <c r="L25" s="12" t="s">
         <v>316</v>
       </c>
     </row>
@@ -7226,13 +7230,13 @@
         <v>258</v>
       </c>
       <c r="I26" s="1"/>
-      <c r="J26" s="11" t="s">
+      <c r="J26" s="12" t="s">
         <v>321</v>
       </c>
       <c r="K26" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="L26" s="11" t="s">
+      <c r="L26" s="12" t="s">
         <v>323</v>
       </c>
     </row>
@@ -7264,13 +7268,13 @@
       <c r="I27" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="J27" s="11" t="s">
+      <c r="J27" s="12" t="s">
         <v>328</v>
       </c>
       <c r="K27" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="L27" s="11" t="s">
+      <c r="L27" s="12" t="s">
         <v>329</v>
       </c>
     </row>
@@ -7328,13 +7332,13 @@
       <c r="I29" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="J29" s="11" t="s">
+      <c r="J29" s="12" t="s">
         <v>337</v>
       </c>
       <c r="K29" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="L29" s="11" t="s">
+      <c r="L29" s="12" t="s">
         <v>338</v>
       </c>
     </row>
@@ -7366,13 +7370,13 @@
       <c r="I30" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="J30" s="11" t="s">
+      <c r="J30" s="12" t="s">
         <v>342</v>
       </c>
       <c r="K30" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="L30" s="11" t="s">
+      <c r="L30" s="12" t="s">
         <v>344</v>
       </c>
     </row>
@@ -7404,13 +7408,13 @@
       <c r="I31" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="J31" s="11" t="s">
+      <c r="J31" s="12" t="s">
         <v>347</v>
       </c>
       <c r="K31" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="L31" s="11" t="s">
+      <c r="L31" s="12" t="s">
         <v>349</v>
       </c>
     </row>
@@ -7442,7 +7446,7 @@
       <c r="I32" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="J32" s="11" t="s">
+      <c r="J32" s="12" t="s">
         <v>353</v>
       </c>
       <c r="K32" s="1" t="s">
@@ -7474,13 +7478,13 @@
       <c r="H33" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="J33" s="11" t="s">
+      <c r="J33" s="12" t="s">
         <v>356</v>
       </c>
       <c r="K33" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="L33" s="11" t="s">
+      <c r="L33" s="12" t="s">
         <v>358</v>
       </c>
     </row>
@@ -7509,13 +7513,13 @@
       <c r="H34" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="J34" s="11" t="s">
+      <c r="J34" s="12" t="s">
         <v>361</v>
       </c>
       <c r="K34" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="L34" s="11" t="s">
+      <c r="L34" s="12" t="s">
         <v>362</v>
       </c>
     </row>
@@ -7547,13 +7551,13 @@
       <c r="I35" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="J35" s="11" t="s">
+      <c r="J35" s="12" t="s">
         <v>367</v>
       </c>
       <c r="K35" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="L35" s="11" t="s">
+      <c r="L35" s="12" t="s">
         <v>369</v>
       </c>
     </row>
@@ -7582,13 +7586,13 @@
       <c r="I36" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="J36" s="11" t="s">
+      <c r="J36" s="12" t="s">
         <v>375</v>
       </c>
       <c r="K36" s="1" t="s">
         <v>376</v>
       </c>
-      <c r="L36" s="11" t="s">
+      <c r="L36" s="12" t="s">
         <v>377</v>
       </c>
     </row>
@@ -7620,13 +7624,13 @@
       <c r="I37" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="J37" s="11" t="s">
+      <c r="J37" s="12" t="s">
         <v>384</v>
       </c>
       <c r="K37" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="L37" s="11" t="s">
+      <c r="L37" s="12" t="s">
         <v>386</v>
       </c>
     </row>
@@ -7652,13 +7656,13 @@
       <c r="H38" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="J38" s="11" t="s">
+      <c r="J38" s="12" t="s">
         <v>389</v>
       </c>
       <c r="K38" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="L38" s="11" t="s">
+      <c r="L38" s="12" t="s">
         <v>391</v>
       </c>
     </row>
@@ -7687,7 +7691,7 @@
       <c r="I39" s="1" t="s">
         <v>395</v>
       </c>
-      <c r="J39" s="11" t="s">
+      <c r="J39" s="12" t="s">
         <v>396</v>
       </c>
       <c r="K39" s="1" t="s">
@@ -7722,13 +7726,13 @@
       <c r="I40" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="J40" s="11" t="s">
+      <c r="J40" s="12" t="s">
         <v>400</v>
       </c>
       <c r="K40" s="1" t="s">
         <v>401</v>
       </c>
-      <c r="L40" s="11" t="s">
+      <c r="L40" s="12" t="s">
         <v>402</v>
       </c>
     </row>
@@ -7757,16 +7761,16 @@
       <c r="H41" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="I41" s="15" t="s">
+      <c r="I41" s="16" t="s">
         <v>404</v>
       </c>
-      <c r="J41" s="11" t="s">
+      <c r="J41" s="12" t="s">
         <v>405</v>
       </c>
       <c r="K41" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="L41" s="11" t="s">
+      <c r="L41" s="12" t="s">
         <v>407</v>
       </c>
     </row>
@@ -7863,14 +7867,14 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B3" activeCellId="1" sqref="A22:F23 B3"/>
+      <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="6" width="11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="6" width="25.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="6" width="48.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="7" width="25.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="7" width="48.75"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7956,7 +7960,7 @@
       <c r="G3" s="1" t="s">
         <v>424</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="12" t="s">
         <v>425</v>
       </c>
       <c r="I3" s="1" t="n">
@@ -8017,7 +8021,7 @@
       <c r="G5" s="1" t="s">
         <v>424</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="H5" s="12" t="s">
         <v>425</v>
       </c>
       <c r="I5" s="1" t="n">
@@ -8078,7 +8082,7 @@
       <c r="G7" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="H7" s="12" t="s">
         <v>425</v>
       </c>
       <c r="I7" s="1" t="n">
@@ -8168,7 +8172,7 @@
       <c r="G10" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="H10" s="12" t="s">
         <v>435</v>
       </c>
       <c r="I10" s="1" t="n">
@@ -8229,7 +8233,7 @@
       <c r="G12" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="H12" s="11" t="s">
+      <c r="H12" s="12" t="s">
         <v>437</v>
       </c>
       <c r="I12" s="1" t="n">
@@ -8261,7 +8265,7 @@
       <c r="G13" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="H13" s="11" t="s">
+      <c r="H13" s="12" t="s">
         <v>439</v>
       </c>
       <c r="I13" s="1" t="n">
@@ -8293,7 +8297,7 @@
       <c r="G14" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="H14" s="11" t="s">
+      <c r="H14" s="12" t="s">
         <v>425</v>
       </c>
       <c r="I14" s="1" t="n">
@@ -8325,7 +8329,7 @@
       <c r="G15" s="1" t="s">
         <v>431</v>
       </c>
-      <c r="H15" s="11" t="s">
+      <c r="H15" s="12" t="s">
         <v>440</v>
       </c>
       <c r="I15" s="1" t="n">
@@ -8380,7 +8384,7 @@
       <c r="G17" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="H17" s="11" t="s">
+      <c r="H17" s="12" t="s">
         <v>437</v>
       </c>
     </row>
@@ -8406,7 +8410,7 @@
       <c r="G18" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="H18" s="11" t="s">
+      <c r="H18" s="12" t="s">
         <v>439</v>
       </c>
     </row>

</xml_diff>